<commit_message>
CHANGE Miilon - Add two more sections on the page 61.
</commit_message>
<xml_diff>
--- a/MiilonData/06_EditoB2_unite4_p61_La_geographie.xlsx
+++ b/MiilonData/06_EditoB2_unite4_p61_La_geographie.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GÉNÉRALITÉS" sheetId="1" r:id="rId1"/>
+    <sheet name="LE PAYS" sheetId="2" r:id="rId2"/>
+    <sheet name="LE RELIEF ET LA VÉGÉTATION" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="148">
   <si>
     <t>Mot français</t>
   </si>
@@ -282,6 +284,192 @@
   </si>
   <si>
     <t>tropický</t>
+  </si>
+  <si>
+    <t>capitale</t>
+  </si>
+  <si>
+    <t>kapital</t>
+  </si>
+  <si>
+    <t>hlavní město</t>
+  </si>
+  <si>
+    <t>frontière</t>
+  </si>
+  <si>
+    <t>fro~tje:r</t>
+  </si>
+  <si>
+    <t>hranice</t>
+  </si>
+  <si>
+    <t>indigène</t>
+  </si>
+  <si>
+    <t>e~dižen</t>
+  </si>
+  <si>
+    <t>domorodý, tuzemský, domácí</t>
+  </si>
+  <si>
+    <t>peuplement</t>
+  </si>
+  <si>
+    <t>zalidnění</t>
+  </si>
+  <si>
+    <t>pöpl@ma~</t>
+  </si>
+  <si>
+    <t>peupler</t>
+  </si>
+  <si>
+    <t>vt</t>
+  </si>
+  <si>
+    <t>pöple.</t>
+  </si>
+  <si>
+    <t>zalidnit, obývat</t>
+  </si>
+  <si>
+    <t>région</t>
+  </si>
+  <si>
+    <t>re.žjo~</t>
+  </si>
+  <si>
+    <t>oblast</t>
+  </si>
+  <si>
+    <t>territoire</t>
+  </si>
+  <si>
+    <t>teritu^a:r</t>
+  </si>
+  <si>
+    <t>území</t>
+  </si>
+  <si>
+    <t>désert</t>
+  </si>
+  <si>
+    <t>de.ze:r</t>
+  </si>
+  <si>
+    <t>pustina, poušť</t>
+  </si>
+  <si>
+    <t>désertique</t>
+  </si>
+  <si>
+    <t>de.zertik</t>
+  </si>
+  <si>
+    <t>pouštní</t>
+  </si>
+  <si>
+    <t>forestier, ière</t>
+  </si>
+  <si>
+    <t>forestje., stje:r</t>
+  </si>
+  <si>
+    <t>lesní, lesnický</t>
+  </si>
+  <si>
+    <t>forêt</t>
+  </si>
+  <si>
+    <t>fore</t>
+  </si>
+  <si>
+    <t>les</t>
+  </si>
+  <si>
+    <t>jungle</t>
+  </si>
+  <si>
+    <t>žo~:gl, žö~:gl</t>
+  </si>
+  <si>
+    <t>džungle</t>
+  </si>
+  <si>
+    <t>oasis</t>
+  </si>
+  <si>
+    <t>oazis</t>
+  </si>
+  <si>
+    <t>oáza</t>
+  </si>
+  <si>
+    <t>plaine</t>
+  </si>
+  <si>
+    <t>plen</t>
+  </si>
+  <si>
+    <t>rovina, planina</t>
+  </si>
+  <si>
+    <t>plateau</t>
+  </si>
+  <si>
+    <t>plato.</t>
+  </si>
+  <si>
+    <t>plošina, náhorní rovina</t>
+  </si>
+  <si>
+    <t>pôle</t>
+  </si>
+  <si>
+    <t>po:l</t>
+  </si>
+  <si>
+    <t>pól</t>
+  </si>
+  <si>
+    <t>prairie</t>
+  </si>
+  <si>
+    <t>preri</t>
+  </si>
+  <si>
+    <t>louka, prérie</t>
+  </si>
+  <si>
+    <t>rural, ale, aux</t>
+  </si>
+  <si>
+    <t>rüral</t>
+  </si>
+  <si>
+    <t>polní, venkovský</t>
+  </si>
+  <si>
+    <t>savane</t>
+  </si>
+  <si>
+    <t>savan</t>
+  </si>
+  <si>
+    <t>savana</t>
+  </si>
+  <si>
+    <t>sol</t>
+  </si>
+  <si>
+    <t>půda, země</t>
+  </si>
+  <si>
+    <t>steppe</t>
+  </si>
+  <si>
+    <t>step</t>
   </si>
 </sst>
 </file>
@@ -631,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,4 +1352,452 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="63" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "capitale", "grammar": "nf", "pronunciation": "kapital", "meaning": "hlavní město" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F8" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "frontière", "grammar": "nf", "pronunciation": "fro~tje:r", "meaning": "hranice" },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "indigène", "grammar": "adj", "pronunciation": "e~dižen", "meaning": "domorodý, tuzemský, domácí" },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "peuplement", "grammar": "nm", "pronunciation": "pöpl@ma~", "meaning": "zalidnění" },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "peupler", "grammar": "vt", "pronunciation": "pöple.", "meaning": "zalidnit, obývat" },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "région", "grammar": "nf", "pronunciation": "re.žjo~", "meaning": "oblast" },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "territoire", "grammar": "nm", "pronunciation": "teritu^a:r", "meaning": "území" },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" t="str">
+        <f xml:space="preserve"> "{ ""foreign"": """ &amp; A2 &amp; """, ""grammar"": """ &amp; B2 &amp; """, ""pronunciation"": """ &amp; C2 &amp; """, ""meaning"": """ &amp; D2 &amp; """ },"</f>
+        <v>{ "foreign": "désert", "grammar": "nm", "pronunciation": "de.ze:r", "meaning": "pustina, poušť" },</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F15" si="0" xml:space="preserve"> "{ ""foreign"": """ &amp; A3 &amp; """, ""grammar"": """ &amp; B3 &amp; """, ""pronunciation"": """ &amp; C3 &amp; """, ""meaning"": """ &amp; D3 &amp; """ },"</f>
+        <v>{ "foreign": "désertique", "grammar": "adj", "pronunciation": "de.zertik", "meaning": "pouštní" },</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "forestier, ière", "grammar": "adj", "pronunciation": "forestje., stje:r", "meaning": "lesní, lesnický" },</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "forêt", "grammar": "nf", "pronunciation": "fore", "meaning": "les" },</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "jungle", "grammar": "nf", "pronunciation": "žo~:gl, žö~:gl", "meaning": "džungle" },</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "oasis", "grammar": "nf", "pronunciation": "oazis", "meaning": "oáza" },</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "plaine", "grammar": "nf", "pronunciation": "plen", "meaning": "rovina, planina" },</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "plateau", "grammar": "nm", "pronunciation": "plato.", "meaning": "plošina, náhorní rovina" },</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "pôle", "grammar": "nm", "pronunciation": "po:l", "meaning": "pól" },</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "prairie", "grammar": "nf", "pronunciation": "preri", "meaning": "louka, prérie" },</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "rural, ale, aux", "grammar": "adj", "pronunciation": "rüral", "meaning": "polní, venkovský" },</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "savane", "grammar": "nf", "pronunciation": "savan", "meaning": "savana" },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "sol", "grammar": "nm", "pronunciation": "sol", "meaning": "půda, země" },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "foreign": "steppe", "grammar": "nf", "pronunciation": "step", "meaning": "step" },</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>